<commit_message>
perdhesa katet 1 done
</commit_message>
<xml_diff>
--- a/2966-1/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-1-Ferizaj-Armendi-leg.xlsx
+++ b/2966-1/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-1-Ferizaj-Armendi-leg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\925-41-Ferizaj-Leg-Naseri\3-Katet\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-1\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5A495C-01B1-40A0-98A6-F5902B6EBD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622C400-F951-4C5C-8B6B-FE1D4B3C5657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="28440" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="255" windowWidth="27930" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$54</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,6 +507,72 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,72 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="B39:I48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,115 +1260,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="24"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1420,13 +1420,13 @@
       <c r="F15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="34">
         <v>118.2</v>
       </c>
     </row>
@@ -1446,11 +1446,11 @@
       <c r="F16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="33"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>18</v>
       </c>
@@ -1466,11 +1466,11 @@
       <c r="F17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G17" s="33"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>7</v>
       </c>
@@ -1486,11 +1486,11 @@
       <c r="F18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G18" s="33"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>16</v>
       </c>
@@ -1506,11 +1506,11 @@
       <c r="F19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="25"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G19" s="33"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>9</v>
       </c>
@@ -1526,11 +1526,11 @@
       <c r="F20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G20" s="33"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>10</v>
       </c>
@@ -1546,11 +1546,11 @@
       <c r="F21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G21" s="33"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>2</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="F22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="25"/>
+      <c r="G22" s="33"/>
       <c r="H22" s="14" t="s">
         <v>13</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>118.2</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1583,7 +1583,7 @@
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1591,7 +1591,7 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
         <v>5</v>
       </c>
@@ -1616,8 +1616,11 @@
       <c r="I25" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>98.89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>36</v>
       </c>
@@ -1633,17 +1636,20 @@
       <c r="F26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="33">
         <v>109.10299999999999</v>
       </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>15.148</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>42</v>
       </c>
@@ -1659,11 +1665,11 @@
       <c r="F27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>43</v>
       </c>
@@ -1679,11 +1685,11 @@
       <c r="F28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>44</v>
       </c>
@@ -1699,17 +1705,11 @@
       <c r="F29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="Q29">
-        <v>70.033000000000001</v>
-      </c>
-      <c r="R29">
-        <v>42.243000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>58</v>
       </c>
@@ -1725,11 +1725,11 @@
       <c r="F30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>60</v>
       </c>
@@ -1745,11 +1745,11 @@
       <c r="F31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>62</v>
       </c>
@@ -1765,9 +1765,9 @@
       <c r="F32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
@@ -1785,9 +1785,9 @@
       <c r="F33" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
@@ -1805,7 +1805,7 @@
       <c r="F34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="33"/>
       <c r="H34" s="10" t="s">
         <v>14</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="F35" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="25"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
     </row>
@@ -1849,7 +1849,7 @@
       <c r="F36" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="25"/>
+      <c r="G36" s="33"/>
       <c r="H36" s="14" t="s">
         <v>13</v>
       </c>
@@ -1916,13 +1916,13 @@
       <c r="F40" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G40" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="25">
+      <c r="I40" s="33">
         <v>70.03</v>
       </c>
     </row>
@@ -1942,9 +1942,9 @@
       <c r="F41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
@@ -1962,9 +1962,9 @@
       <c r="F42" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
@@ -1982,9 +1982,9 @@
       <c r="F43" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
@@ -2002,9 +2002,9 @@
       <c r="F44" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
@@ -2022,9 +2022,9 @@
       <c r="F45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
@@ -2042,7 +2042,7 @@
       <c r="F46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="25"/>
+      <c r="G46" s="33"/>
       <c r="H46" s="10" t="s">
         <v>14</v>
       </c>
@@ -2066,7 +2066,7 @@
       <c r="F47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="25"/>
+      <c r="G47" s="33"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
     </row>
@@ -2086,7 +2086,7 @@
       <c r="F48" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="25"/>
+      <c r="G48" s="33"/>
       <c r="H48" s="14" t="s">
         <v>13</v>
       </c>
@@ -2129,34 +2129,34 @@
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="35" t="s">
+      <c r="E53" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="36"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="31" t="s">
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="32"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="27"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="16"/>
     </row>
     <row r="54" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="38" t="s">
+      <c r="A54" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41">
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="30">
         <v>140</v>
       </c>
-      <c r="F54" s="42"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="29"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="18"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K55" s="1"/>
@@ -2169,6 +2169,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="G15:G22"/>
     <mergeCell ref="J53:K54"/>
     <mergeCell ref="A3:K6"/>
     <mergeCell ref="H53:I54"/>
@@ -2183,9 +2186,6 @@
     <mergeCell ref="G40:G48"/>
     <mergeCell ref="H40:H45"/>
     <mergeCell ref="I40:I45"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="C8:J10"/>
-    <mergeCell ref="G15:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
katet done ob 1
</commit_message>
<xml_diff>
--- a/2966-1/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-1-Ferizaj-Armendi-leg.xlsx
+++ b/2966-1/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-1-Ferizaj-Armendi-leg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-1\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622C400-F951-4C5C-8B6B-FE1D4B3C5657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013B0F0F-72B5-479C-9157-9AC100ACFEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="255" windowWidth="27930" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$58</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
   <si>
     <t>Y</t>
   </si>
@@ -85,25 +85,22 @@
     <t>Kati 1</t>
   </si>
   <si>
-    <t>perdhes</t>
-  </si>
-  <si>
-    <t>perdhesa</t>
-  </si>
-  <si>
-    <t>perdhhes</t>
-  </si>
-  <si>
     <t>kati1</t>
   </si>
   <si>
-    <t>kati teras</t>
+    <t>perdhese</t>
   </si>
   <si>
-    <t>Kati NK</t>
+    <t>perdhese-terasa</t>
   </si>
   <si>
-    <t>Kati N</t>
+    <t>bodrum</t>
+  </si>
+  <si>
+    <t>Bodrumi</t>
+  </si>
+  <si>
+    <t>kati1_terasa</t>
   </si>
 </sst>
 </file>
@@ -469,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -507,6 +504,54 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,48 +605,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,115 +1263,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="40"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="44"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="46"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1406,786 +1409,860 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5">
-        <v>7512081.3849999998</v>
+        <v>7510641.8290999997</v>
       </c>
       <c r="D15" s="5">
-        <v>4691786.2439999999</v>
+        <v>4693478.6179</v>
       </c>
       <c r="E15" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="34">
-        <v>118.2</v>
+      <c r="I15" s="28">
+        <v>98.89</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5">
-        <v>7512079.642</v>
+        <v>7510639.7030999996</v>
       </c>
       <c r="D16" s="5">
-        <v>4691779.6717999997</v>
+        <v>4693477.3641999997</v>
       </c>
       <c r="E16" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5">
+        <v>7510639.2317000004</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4693465.7909000004</v>
+      </c>
+      <c r="E17" s="10">
+        <v>648.24800000000005</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
-        <v>7512082.0530000003</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4691766.5650000004</v>
-      </c>
-      <c r="E17" s="10">
-        <v>614.02200000000005</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G17" s="27"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5">
-        <v>7512079.2779999999</v>
+        <v>7510638.0011</v>
       </c>
       <c r="D18" s="5">
-        <v>4691779.7949999999</v>
+        <v>4693465.0647999998</v>
       </c>
       <c r="E18" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5">
-        <v>7512076.6830000002</v>
+        <v>7510632.9046</v>
       </c>
       <c r="D19" s="5">
-        <v>4691768.2429999998</v>
+        <v>4693473.3550000004</v>
       </c>
       <c r="E19" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C20" s="5">
-        <v>7512078.3710000003</v>
+        <v>7510639.2709999997</v>
       </c>
       <c r="D20" s="5">
-        <v>4691775.9160000002</v>
+        <v>4693465.727</v>
       </c>
       <c r="E20" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G20" s="27"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="C21" s="5">
-        <v>7512076.4800000004</v>
+        <v>7510641.0773</v>
       </c>
       <c r="D21" s="5">
-        <v>4691768.6579999998</v>
+        <v>4693466.7927000001</v>
       </c>
       <c r="E21" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G21" s="27"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="C22" s="5">
-        <v>7512087.7089</v>
+        <v>7510641.0379999997</v>
       </c>
       <c r="D22" s="5">
-        <v>4691784.1546999998</v>
+        <v>4693466.8565999996</v>
       </c>
       <c r="E22" s="10">
-        <v>614.02200000000005</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>100</v>
+      </c>
+      <c r="C23" s="5">
+        <v>7510645.0045999996</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4693469.1969999997</v>
+      </c>
+      <c r="E23" s="10">
+        <v>648.24800000000005</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>101</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7510644.6449999996</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4693469.7819999997</v>
+      </c>
+      <c r="E24" s="10">
+        <v>648.24800000000005</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>102</v>
+      </c>
+      <c r="C25" s="5">
+        <v>7510646.4632999999</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4693470.8547999999</v>
+      </c>
+      <c r="E25" s="10">
+        <v>648.24800000000005</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="16">
+        <v>15.148</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
         <v>19</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="14" t="s">
+      <c r="C26" s="5">
+        <v>7510638.7419999996</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4693478.9939999999</v>
+      </c>
+      <c r="E26" s="10">
+        <v>648.21199999999999</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="27"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <v>20</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7510631.8894999996</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4693475.0062999995</v>
+      </c>
+      <c r="E27" s="10">
+        <v>648.24800000000005</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="14">
-        <f>SUM(I15:I21)</f>
-        <v>118.2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
+      <c r="I27" s="14">
+        <f>SUM(I15:I25)</f>
+        <v>114.038</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E30" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H30" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O25">
-        <v>98.89</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="11">
-        <v>36</v>
-      </c>
-      <c r="C26" s="5">
-        <v>7512081.3770000003</v>
-      </c>
-      <c r="D26" s="5">
-        <v>4691786.2220000001</v>
-      </c>
-      <c r="E26" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="33" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7510640.0105999997</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4693477.5455</v>
+      </c>
+      <c r="E31" s="10">
+        <v>651.38900000000001</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H31" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="33">
-        <v>109.10299999999999</v>
-      </c>
-      <c r="O26">
-        <v>15.148</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
-        <v>42</v>
-      </c>
-      <c r="C27" s="5">
-        <v>7512079.642</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4691779.6717999997</v>
-      </c>
-      <c r="E27" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="11">
-        <v>43</v>
-      </c>
-      <c r="C28" s="5">
-        <v>7512076.7105999999</v>
-      </c>
-      <c r="D28" s="5">
-        <v>4691769.5429999996</v>
-      </c>
-      <c r="E28" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="11">
-        <v>44</v>
-      </c>
-      <c r="C29" s="5">
-        <v>7512078.3710000003</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4691775.9160000002</v>
-      </c>
-      <c r="E29" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="11">
-        <v>58</v>
-      </c>
-      <c r="C30" s="5">
-        <v>7512083.0329</v>
-      </c>
-      <c r="D30" s="5">
-        <v>4691769.6122000003</v>
-      </c>
-      <c r="E30" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
-        <v>60</v>
-      </c>
-      <c r="C31" s="5">
-        <v>7512087.7089</v>
-      </c>
-      <c r="D31" s="5">
-        <v>4691784.1546999998</v>
-      </c>
-      <c r="E31" s="10">
-        <v>617.33699999999999</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I31" s="27">
+        <v>79.843000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C32" s="5">
-        <v>7512079.2779999999</v>
+        <v>7510632.9046</v>
       </c>
       <c r="D32" s="5">
-        <v>4691779.7949999999</v>
+        <v>4693473.3550000004</v>
       </c>
       <c r="E32" s="10">
-        <v>617.33699999999999</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
+        <v>17</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C33" s="5">
-        <v>7512081.034</v>
+        <v>7510639.7030999996</v>
       </c>
       <c r="D33" s="5">
-        <v>4691768.2149999999</v>
+        <v>4693477.3641999997</v>
       </c>
       <c r="E33" s="10">
-        <v>617.33699999999999</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+        <v>17</v>
+      </c>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="5">
-        <v>7512082.8425000003</v>
+        <v>7510644.9709999999</v>
       </c>
       <c r="D34" s="5">
-        <v>4691769.6733999997</v>
+        <v>4693469.2079999996</v>
       </c>
       <c r="E34" s="10">
-        <v>617.33699999999999</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="33"/>
-      <c r="H34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="10">
-        <v>9.8309999999999995</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C35" s="5">
-        <v>7512076.3611000003</v>
+        <v>7510641.0379999997</v>
       </c>
       <c r="D35" s="5">
-        <v>4691768.2016000003</v>
+        <v>4693466.8565999996</v>
       </c>
       <c r="E35" s="10">
-        <v>617.33699999999999</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C36" s="5">
-        <v>7512082.0237999996</v>
+        <v>7510641.0789999999</v>
       </c>
       <c r="D36" s="5">
-        <v>4691766.4742000001</v>
+        <v>4693466.79</v>
       </c>
       <c r="E36" s="10">
-        <v>617.33699999999999</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="14">
-        <f>SUM(I26:I34)</f>
-        <v>118.934</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="B37" s="11">
+        <v>70</v>
+      </c>
+      <c r="C37" s="5">
+        <v>7510639.2709999997</v>
+      </c>
+      <c r="D37" s="5">
+        <v>4693465.727</v>
+      </c>
+      <c r="E37" s="10">
+        <v>651.38900000000001</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="B38" s="11">
+        <v>71</v>
+      </c>
+      <c r="C38" s="5">
+        <v>7510639.2317000004</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4693465.7909000004</v>
+      </c>
+      <c r="E38" s="10">
+        <v>651.38900000000001</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>7</v>
+      <c r="B39" s="11">
+        <v>72</v>
+      </c>
+      <c r="C39" s="5">
+        <v>7510638.0011</v>
+      </c>
+      <c r="D39" s="5">
+        <v>4693465.0647999998</v>
+      </c>
+      <c r="E39" s="10">
+        <v>651.38900000000001</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="27"/>
+      <c r="H39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="10">
+        <v>7.6779999999999999</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C40" s="5">
-        <v>7512084.4585999995</v>
+        <v>7510632.3836000003</v>
       </c>
       <c r="D40" s="5">
-        <v>4691774.0460999999</v>
+        <v>4693474.2024999997</v>
       </c>
       <c r="E40" s="10">
-        <v>620.23699999999997</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="I40" s="33">
-        <v>70.03</v>
-      </c>
+      <c r="G40" s="27"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C41" s="5">
-        <v>7512087.7089</v>
+        <v>7510639.2210999997</v>
       </c>
       <c r="D41" s="5">
-        <v>4691784.1546999998</v>
+        <v>4693478.1814999999</v>
       </c>
       <c r="E41" s="10">
-        <v>620.23699999999997</v>
+        <v>651.38900000000001</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
+        <v>22</v>
+      </c>
+      <c r="G41" s="27"/>
+      <c r="H41" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="14">
+        <f>SUM(I31:I39)</f>
+        <v>87.521000000000001</v>
+      </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="11">
-        <v>30</v>
-      </c>
-      <c r="C42" s="5">
-        <v>7512079.642</v>
-      </c>
-      <c r="D42" s="5">
-        <v>4691779.6717999997</v>
-      </c>
-      <c r="E42" s="10">
-        <v>620.23699999999997</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="11">
-        <v>31</v>
-      </c>
-      <c r="C43" s="5">
-        <v>7512078.3710000003</v>
-      </c>
-      <c r="D43" s="5">
-        <v>4691775.9160000002</v>
-      </c>
-      <c r="E43" s="10">
-        <v>620.23699999999997</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="11">
-        <v>33</v>
-      </c>
-      <c r="C44" s="5">
-        <v>7512079.2779999999</v>
-      </c>
-      <c r="D44" s="5">
-        <v>4691779.7949999999</v>
-      </c>
-      <c r="E44" s="10">
-        <v>620.23699999999997</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
+      <c r="B44" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C45" s="5">
-        <v>7512081.3770000003</v>
+        <v>7510632.9242000002</v>
       </c>
       <c r="D45" s="5">
-        <v>4691786.2220000001</v>
+        <v>4693473.3230999997</v>
       </c>
       <c r="E45" s="10">
-        <v>620.23699999999997</v>
+        <v>645.94299999999998</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
+      <c r="G45" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="27">
+        <v>49.24</v>
+      </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C46" s="5">
-        <v>7512076.7105999999</v>
+        <v>7510635.3864000002</v>
       </c>
       <c r="D46" s="5">
-        <v>4691769.5429999996</v>
+        <v>4693469.3180999998</v>
       </c>
       <c r="E46" s="10">
-        <v>620.23699999999997</v>
+        <v>645.94299999999998</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="33"/>
-      <c r="H46" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I46" s="10">
-        <v>42.24</v>
-      </c>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C47" s="5">
-        <v>7512081.034</v>
+        <v>7510639.2479999997</v>
       </c>
       <c r="D47" s="5">
-        <v>4691768.2149999999</v>
+        <v>4693477.085</v>
       </c>
       <c r="E47" s="10">
-        <v>620.23699999999997</v>
+        <v>645.89800000000002</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="33"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="11">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="C48" s="5">
-        <v>7512082.0237999996</v>
+        <v>7510644.2862</v>
       </c>
       <c r="D48" s="5">
-        <v>4691766.4742000001</v>
+        <v>4693474.5017999997</v>
       </c>
       <c r="E48" s="10">
-        <v>620.23699999999997</v>
+        <v>645.94299999999998</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="33"/>
-      <c r="H48" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="11">
+        <v>120</v>
+      </c>
+      <c r="C49" s="5">
+        <v>7510641.7368999999</v>
+      </c>
+      <c r="D49" s="5">
+        <v>4693478.7723000003</v>
+      </c>
+      <c r="E49" s="10">
+        <v>645.94299999999998</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="11">
+        <v>121</v>
+      </c>
+      <c r="C50" s="5">
+        <v>7510639.6945000002</v>
+      </c>
+      <c r="D50" s="5">
+        <v>4693477.5827000001</v>
+      </c>
+      <c r="E50" s="10">
+        <v>645.94299999999998</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="11">
+        <v>122</v>
+      </c>
+      <c r="C51" s="5">
+        <v>7510639.7977999998</v>
+      </c>
+      <c r="D51" s="5">
+        <v>4693477.4052999998</v>
+      </c>
+      <c r="E51" s="10">
+        <v>645.94299999999998</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="27"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="11">
+        <v>123</v>
+      </c>
+      <c r="C52" s="5">
+        <v>7510639.2822000002</v>
+      </c>
+      <c r="D52" s="5">
+        <v>4693477.0263</v>
+      </c>
+      <c r="E52" s="10">
+        <v>645.94299999999998</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="27"/>
+      <c r="H52" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I48" s="14">
-        <f>SUM(I40:I46)</f>
-        <v>112.27000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="6"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="6"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-    </row>
-    <row r="52" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K52" s="1"/>
-    </row>
-    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="I52" s="14">
+        <f>SUM(I45:I50)</f>
+        <v>49.24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="24" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="25"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="20" t="s">
+      <c r="F57" s="41"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="16"/>
-    </row>
-    <row r="54" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="27" t="s">
+      <c r="I57" s="37"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="32"/>
+    </row>
+    <row r="58" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30">
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="46">
         <v>140</v>
       </c>
-      <c r="F54" s="31"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="18"/>
-    </row>
-    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K55" s="1"/>
-    </row>
-    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K56" s="1"/>
-    </row>
-    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K57" s="1"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="34"/>
+    </row>
+    <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K61" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J57:K58"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="H57:I58"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="G31:G41"/>
+    <mergeCell ref="H31:H38"/>
+    <mergeCell ref="I31:I38"/>
+    <mergeCell ref="G45:G52"/>
+    <mergeCell ref="H45:H50"/>
+    <mergeCell ref="I45:I50"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="C8:J10"/>
-    <mergeCell ref="G15:G22"/>
-    <mergeCell ref="J53:K54"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H53:I54"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="G26:G36"/>
-    <mergeCell ref="H26:H33"/>
-    <mergeCell ref="I26:I33"/>
-    <mergeCell ref="H15:H21"/>
-    <mergeCell ref="I15:I21"/>
-    <mergeCell ref="G40:G48"/>
-    <mergeCell ref="H40:H45"/>
-    <mergeCell ref="I40:I45"/>
+    <mergeCell ref="G15:G27"/>
+    <mergeCell ref="H15:H24"/>
+    <mergeCell ref="I15:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>